<commit_message>
Started changing to KUBE setup
</commit_message>
<xml_diff>
--- a/CoA.xlsx
+++ b/CoA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onedrive-global.kpmg.com/personal/jsteensgaard_kpmg_com/Documents/Documents/Synthetic_Data_Generation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{33B732EC-9ED0-44F0-B9AD-CEE0EF80052E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55411496-4639-4D73-8B02-83547D23C5A1}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{33B732EC-9ED0-44F0-B9AD-CEE0EF80052E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC14F3FB-9CC2-5B45-B953-7B4F2E3CA539}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3BEE8EC9-D0E2-44BB-A1C8-8055F112EC32}"/>
   </bookViews>

</xml_diff>